<commit_message>
Update full model unit tests
</commit_message>
<xml_diff>
--- a/tests/cascade_spreadsheet/cascade_model_full.xlsx
+++ b/tests/cascade_spreadsheet/cascade_model_full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16005" windowHeight="5730" tabRatio="647"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16005" windowHeight="5730" tabRatio="647" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="139">
   <si>
     <t>Code Label</t>
   </si>
@@ -432,6 +432,15 @@
   </si>
   <si>
     <t>Epidemic Characteristics</t>
+  </si>
+  <si>
+    <t>avg_contacts_in</t>
+  </si>
+  <si>
+    <t>i_rate/100</t>
+  </si>
+  <si>
+    <t>i_rate/50</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1652,7 +1661,7 @@
       <c r="A5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="24" t="s">
         <v>63</v>
       </c>
       <c r="L5" s="8"/>
@@ -1764,7 +1773,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,10 +2323,16 @@
         <v>125</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2354,10 +2369,13 @@
         <v>125</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2554,10 +2572,13 @@
         <v>125</v>
       </c>
       <c r="F15" s="2">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Scenario Unit Test left
</commit_message>
<xml_diff>
--- a/tests/cascade_spreadsheet/cascade_model_full.xlsx
+++ b/tests/cascade_spreadsheet/cascade_model_full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16005" windowHeight="5730" tabRatio="647" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16005" windowHeight="5730" tabRatio="647" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="139">
   <si>
     <t>Code Label</t>
   </si>
@@ -1772,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,9 +1854,6 @@
       <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1877,9 +1874,6 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="H3" s="2" t="s">
         <v>48</v>
       </c>
@@ -1923,9 +1917,6 @@
       <c r="D5" s="2">
         <v>2</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="H5" s="2" t="s">
         <v>68</v>
       </c>
@@ -1946,9 +1937,6 @@
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="H6" s="2" t="s">
         <v>70</v>
       </c>
@@ -1969,9 +1957,6 @@
       <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="H7" s="2" t="s">
         <v>69</v>
       </c>
@@ -1991,9 +1976,6 @@
       </c>
       <c r="D8" s="2">
         <v>5</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>71</v>
@@ -2238,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showWhiteSpace="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Complete scenarios and project testing
</commit_message>
<xml_diff>
--- a/tests/cascade_spreadsheet/cascade_model_full.xlsx
+++ b/tests/cascade_spreadsheet/cascade_model_full.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="145">
   <si>
     <t>Code Label</t>
   </si>
@@ -441,6 +441,24 @@
   </si>
   <si>
     <t>i_rate/50</t>
+  </si>
+  <si>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>Number of births</t>
+  </si>
+  <si>
+    <t>ad_inf</t>
+  </si>
+  <si>
+    <t>Total number of DS Infections</t>
+  </si>
+  <si>
+    <t>am_inf</t>
+  </si>
+  <si>
+    <t>Total number of MDR Infections</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1581,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,137 +2004,117 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="D9" s="2">
         <v>-1</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="K9" t="s">
-        <v>92</v>
-      </c>
-      <c r="L9" t="s">
-        <v>93</v>
-      </c>
-      <c r="M9" t="s">
         <v>80</v>
-      </c>
-      <c r="N9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="J10" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" t="s">
-        <v>79</v>
-      </c>
-      <c r="M10" t="s">
-        <v>78</v>
-      </c>
-      <c r="N10" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D11" s="2">
         <v>-1</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" t="s">
         <v>92</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="L11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D12" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" t="s">
+        <v>79</v>
+      </c>
+      <c r="M12" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="D13" s="2">
         <v>-1</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I13" t="s">
-        <v>13</v>
-      </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2124,7 +2122,7 @@
         <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D14" s="2">
         <v>-1</v>
@@ -2141,16 +2139,14 @@
       <c r="J14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D15" s="2">
         <v>-1</v>
@@ -2167,16 +2163,14 @@
       <c r="J15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2">
         <v>-1</v>
@@ -2191,23 +2185,98 @@
         <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D17" s="2">
         <v>-1</v>
       </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J17" t="s">
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2221,7 +2290,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>